<commit_message>
updated import code and images
</commit_message>
<xml_diff>
--- a/code/actions/Projects.xlsx
+++ b/code/actions/Projects.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\code\actions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7C1AB5-A3A3-4875-B124-8471E2A56292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77E47A2-46D0-4D35-AC1C-76386D3775B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="3690" windowWidth="28800" windowHeight="15540" xr2:uid="{1752FA05-084F-4C8E-9E39-6850F815556A}"/>
+    <workbookView xWindow="15" yWindow="1110" windowWidth="28785" windowHeight="15090" xr2:uid="{1752FA05-084F-4C8E-9E39-6850F815556A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="9">
   <si>
     <t>CANEST</t>
   </si>
@@ -412,18 +413,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{063DFC5A-6431-479A-AF53-D4E145D4893A}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -437,7 +438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>6160487</v>
       </c>
@@ -451,7 +452,7 @@
         <v>115.8849578</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6161836</v>
       </c>
@@ -465,7 +466,7 @@
         <v>115.9421</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6161837</v>
       </c>
@@ -479,7 +480,7 @@
         <v>115.9011825</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6161838</v>
       </c>
@@ -493,7 +494,7 @@
         <v>115.8722331</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6161892</v>
       </c>
@@ -507,7 +508,7 @@
         <v>115.9277438</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6162994</v>
       </c>
@@ -521,7 +522,7 @@
         <v>115.9210023</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6162995</v>
       </c>
@@ -535,7 +536,7 @@
         <v>115.91564270000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6163105</v>
       </c>
@@ -549,7 +550,7 @@
         <v>115.9267</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6163119</v>
       </c>
@@ -563,7 +564,7 @@
         <v>115.949901</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6163124</v>
       </c>
@@ -577,7 +578,7 @@
         <v>115.93313120000001</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6163126</v>
       </c>
@@ -591,7 +592,7 @@
         <v>115.94424480000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6163132</v>
       </c>
@@ -605,7 +606,7 @@
         <v>115.9378279</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6163179</v>
       </c>
@@ -619,7 +620,7 @@
         <v>115.853516</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6163346</v>
       </c>
@@ -633,7 +634,7 @@
         <v>115.9155591</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6164609</v>
       </c>
@@ -647,7 +648,7 @@
         <v>115.9132224</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6165318</v>
       </c>
@@ -661,7 +662,7 @@
         <v>115.8532247</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6167188</v>
       </c>
@@ -675,1142 +676,2291 @@
         <v>115.901366</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>6147030</v>
+        <v>6160118</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>-32.156600179999998</v>
+        <v>-31.87807475</v>
       </c>
       <c r="D19">
-        <v>115.70272919999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.99227759999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6147031</v>
+        <v>6160119</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>-32.250800060000003</v>
+        <v>-31.868417000000001</v>
       </c>
       <c r="D20">
-        <v>115.7283213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.99898330000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>6147032</v>
+        <v>6160121</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>-32.19228159</v>
+        <v>-31.891316419999999</v>
       </c>
       <c r="D21">
-        <v>115.74524959999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.97515919999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>6147033</v>
+        <v>6160258</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>-32.272864929999997</v>
+        <v>-32.017126040000001</v>
       </c>
       <c r="D22">
-        <v>115.70268040000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.7841286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>6147034</v>
+        <v>6160259</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23">
-        <v>-32.262401539999999</v>
+        <v>-32.007068689999997</v>
       </c>
       <c r="D23">
-        <v>115.714178</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.80894979999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>6147035</v>
+        <v>6160262</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24">
-        <v>-32.200119899999997</v>
+        <v>-31.96365737</v>
       </c>
       <c r="D24">
-        <v>115.7406544</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.8487799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>6147036</v>
+        <v>6160263</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>-32.157431269999996</v>
+        <v>-31.954845290000002</v>
       </c>
       <c r="D25">
-        <v>115.67930389999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.88534110000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>6147037</v>
+        <v>6160764</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C26">
-        <v>-32.186697510000002</v>
+        <v>-31.939806950000001</v>
       </c>
       <c r="D26">
-        <v>115.7598478</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9081728</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>6141432</v>
+        <v>6160930</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27">
-        <v>-32.274500000000003</v>
+        <v>-31.887653799999999</v>
       </c>
       <c r="D27">
-        <v>115.7025</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.97964109999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>6142830</v>
+        <v>6161086</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>-32.140023960000001</v>
+        <v>-31.86440399</v>
       </c>
       <c r="D28">
-        <v>115.762558</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.00908269999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>6142971</v>
+        <v>6161821</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29">
-        <v>-32.152366469999997</v>
+        <v>-31.912582149999999</v>
       </c>
       <c r="D29">
-        <v>115.72015759999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.96102639999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>6142972</v>
+        <v>6161854</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C30">
-        <v>-32.146479720000002</v>
+        <v>-31.88785918</v>
       </c>
       <c r="D30">
-        <v>115.75672400000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.98954620000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>6142973</v>
+        <v>6161869</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>-32.17070253</v>
+        <v>-31.994891920000001</v>
       </c>
       <c r="D31">
-        <v>115.76248270000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.8353486</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>6142974</v>
+        <v>6161870</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C32">
-        <v>-32.197565330000003</v>
+        <v>-31.951371819999999</v>
       </c>
       <c r="D32">
-        <v>115.7198329</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9134004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>6142975</v>
+        <v>6161878</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C33">
-        <v>-32.209850520000003</v>
+        <v>-31.92140375</v>
       </c>
       <c r="D33">
-        <v>115.75956549999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9401324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>6142976</v>
+        <v>6161879</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C34">
-        <v>-32.238933729999999</v>
+        <v>-31.898440279999999</v>
       </c>
       <c r="D34">
-        <v>115.75141189999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.95925010000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>6142977</v>
+        <v>6162045</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35">
-        <v>-32.256500250000002</v>
+        <v>-31.904372590000001</v>
       </c>
       <c r="D35">
-        <v>115.7408638</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9632125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>6142980</v>
+        <v>6162300</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36">
-        <v>-32.229518179999999</v>
+        <v>-31.90048101</v>
       </c>
       <c r="D36">
-        <v>115.6979693</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9616911</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>6142983</v>
+        <v>6163485</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C37">
-        <v>-32.248231529999998</v>
+        <v>-31.92268434</v>
       </c>
       <c r="D37">
-        <v>115.7125308</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9509489</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>6142984</v>
+        <v>6163500</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C38">
-        <v>-32.182802690000003</v>
+        <v>-31.856300000000001</v>
       </c>
       <c r="D38">
-        <v>115.73908969999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9956</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>6142987</v>
+        <v>6163833</v>
       </c>
       <c r="B39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>-32.254698220000002</v>
+        <v>-31.8614</v>
       </c>
       <c r="D39">
-        <v>115.7401668</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.0027</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>6142988</v>
+        <v>6163857</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40">
-        <v>-32.215296930000001</v>
+        <v>-31.883876350000001</v>
       </c>
       <c r="D40">
-        <v>115.6966123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9912491</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>6142989</v>
+        <v>6163932</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C41">
-        <v>-32.198595249999997</v>
+        <v>-31.8811</v>
       </c>
       <c r="D41">
-        <v>115.6848308</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9913</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>6147030</v>
+        <v>6164323</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C42">
-        <v>-32.156600179999998</v>
+        <v>-31.920072179999998</v>
       </c>
       <c r="D42">
-        <v>115.70272919999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9416183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>6147031</v>
+        <v>6167114</v>
       </c>
       <c r="B43" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>-32.250800060000003</v>
+        <v>-31.894387349999999</v>
       </c>
       <c r="D43">
-        <v>115.7283213</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.9713321</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>6147034</v>
+        <v>6167160</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>-32.262401539999999</v>
+        <v>-31.99888889</v>
       </c>
       <c r="D44">
-        <v>115.714178</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.84425</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>6147035</v>
+        <v>616011</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>-32.200119899999997</v>
+        <v>-31.750532184000001</v>
       </c>
       <c r="D45">
-        <v>115.7406544</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.068524205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>6160118</v>
+        <v>616018</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C46">
-        <v>-31.87807475</v>
+        <v>-31.935681366000001</v>
       </c>
       <c r="D46">
-        <v>115.99227759999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.068640066</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>6160119</v>
+        <v>616027</v>
       </c>
       <c r="B47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C47">
-        <v>-31.868417000000001</v>
+        <v>-32.092304540999997</v>
       </c>
       <c r="D47">
-        <v>115.99898330000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.016771762</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>6160121</v>
+        <v>616042</v>
       </c>
       <c r="B48" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C48">
-        <v>-31.891316419999999</v>
+        <v>-32.025406175999997</v>
       </c>
       <c r="D48">
-        <v>115.97515919999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.96714599400001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>6160258</v>
+        <v>616043</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49">
-        <v>-32.017126040000001</v>
+        <v>-32.016546245999997</v>
       </c>
       <c r="D49">
-        <v>115.7841286</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.919365919</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>6160259</v>
+        <v>616047</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50">
-        <v>-32.007068689999997</v>
+        <v>-32.043205200000003</v>
       </c>
       <c r="D50">
-        <v>115.80894979999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.976086392</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>6160262</v>
+        <v>6160712</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51">
-        <v>-31.96365737</v>
+        <v>-31.795719999999999</v>
       </c>
       <c r="D51">
-        <v>115.8487799</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.0047</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>6160263</v>
+        <v>616076</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C52">
-        <v>-31.954845290000002</v>
+        <v>-31.781684749</v>
       </c>
       <c r="D52">
-        <v>115.88534110000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.022903611</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>6160764</v>
+        <v>616082</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C53">
-        <v>-31.939806950000001</v>
+        <v>-31.924002425000001</v>
       </c>
       <c r="D53">
-        <v>115.9081728</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.92193885899999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>6160930</v>
+        <v>616084</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C54">
-        <v>-31.887653799999999</v>
+        <v>-31.877702540000001</v>
       </c>
       <c r="D54">
-        <v>115.97964109999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.95952564</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>6161086</v>
+        <v>616086</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C55">
-        <v>-31.86440399</v>
+        <v>-31.900081093000001</v>
       </c>
       <c r="D55">
-        <v>116.00908269999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.007611462</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>6161821</v>
+        <v>616087</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C56">
-        <v>-31.912582149999999</v>
+        <v>-31.94828296</v>
       </c>
       <c r="D56">
-        <v>115.96102639999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.91931938</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>6161854</v>
+        <v>616088</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C57">
-        <v>-31.88785918</v>
+        <v>-31.862700963999998</v>
       </c>
       <c r="D57">
-        <v>115.98954620000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.013984561</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>6161869</v>
+        <v>616089</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58">
-        <v>-31.994891920000001</v>
+        <v>-31.821230719999999</v>
       </c>
       <c r="D58">
-        <v>115.8353486</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.12921548</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>6161870</v>
+        <v>616091</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C59">
-        <v>-31.951371819999999</v>
+        <v>-32.038305649999998</v>
       </c>
       <c r="D59">
-        <v>115.9134004</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.91732057</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>6161878</v>
+        <v>616092</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>-31.92140375</v>
+        <v>-32.078355232</v>
       </c>
       <c r="D60">
-        <v>115.9401324</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.978799149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>6161879</v>
+        <v>616099</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>-31.898440279999999</v>
+        <v>-31.817711536000001</v>
       </c>
       <c r="D61">
-        <v>115.95925010000001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.01405090999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>6162045</v>
+        <v>6161013</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>-31.904372590000001</v>
+        <v>-31.820768780000002</v>
       </c>
       <c r="D62">
-        <v>115.9632125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.1276349</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>6162300</v>
+        <v>616178</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63">
-        <v>-31.90048101</v>
+        <v>-31.883961190000001</v>
       </c>
       <c r="D63">
-        <v>115.9616911</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.09479099000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>6163485</v>
+        <v>616189</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64">
-        <v>-31.92268434</v>
+        <v>-31.751071324000002</v>
       </c>
       <c r="D64">
-        <v>115.9509489</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.024830094</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>6163500</v>
+        <v>6161989</v>
       </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65">
-        <v>-31.856300000000001</v>
+        <v>-32.096312699999999</v>
       </c>
       <c r="D65">
-        <v>115.9956</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.017131529</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>6163833</v>
+        <v>6162924</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66">
-        <v>-31.8614</v>
+        <v>-32.033500109999999</v>
       </c>
       <c r="D66">
-        <v>116.0027</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.00569905</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>6163857</v>
+        <v>6162925</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>-31.883876350000001</v>
+        <v>-31.876150470999999</v>
       </c>
       <c r="D67">
-        <v>115.9912491</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.017298422</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>6163932</v>
+        <v>6163143</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68">
-        <v>-31.8811</v>
+        <v>-31.87541667</v>
       </c>
       <c r="D68">
-        <v>115.9913</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.95690878000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>6164323</v>
+        <v>6163625</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69">
-        <v>-31.920072179999998</v>
+        <v>-31.800609914999999</v>
       </c>
       <c r="D69">
-        <v>115.9416183</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.999476379</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>6167114</v>
+        <v>6163713</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70">
-        <v>-31.894387349999999</v>
+        <v>-31.952680231999999</v>
       </c>
       <c r="D70">
-        <v>115.9713321</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.880203943</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>6167160</v>
+        <v>6164314</v>
       </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>-31.99888889</v>
+        <v>-31.78947681</v>
       </c>
       <c r="D71">
-        <v>115.84425</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+        <v>116.00394692</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>616011</v>
+        <v>6164462</v>
       </c>
       <c r="B72" t="s">
         <v>3</v>
       </c>
       <c r="C72">
-        <v>-31.750532184000001</v>
+        <v>-31.949030721</v>
       </c>
       <c r="D72">
-        <v>116.068524205</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.91973172500001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>616018</v>
+        <v>6140304</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73">
-        <v>-31.935681366000001</v>
+        <v>-32.257826999999999</v>
       </c>
       <c r="D73">
-        <v>116.068640066</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.710932</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>616027</v>
+        <v>6140305</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74">
-        <v>-32.092304540999997</v>
+        <v>-32.257826999999999</v>
       </c>
       <c r="D74">
-        <v>116.016771762</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.710932</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>616042</v>
+        <v>6140789</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>-32.025406175999997</v>
+        <v>-32.276461855999997</v>
       </c>
       <c r="D75">
-        <v>115.96714599400001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.72685915700001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>616043</v>
+        <v>6140790</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76">
-        <v>-32.016546245999997</v>
+        <v>-32.248224673999999</v>
       </c>
       <c r="D76">
-        <v>115.919365919</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.75642224400001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>616047</v>
+        <v>6140791</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77">
-        <v>-32.043205200000003</v>
+        <v>-32.182937180000003</v>
       </c>
       <c r="D77">
-        <v>115.976086392</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.775268369</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>6160712</v>
+        <v>6140801</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78">
-        <v>-31.795719999999999</v>
+        <v>-32.140373017000002</v>
       </c>
       <c r="D78">
-        <v>116.0047</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.762744056</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>616076</v>
+        <v>6140802</v>
       </c>
       <c r="B79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79">
-        <v>-31.781684749</v>
+        <v>-32.139167512999997</v>
       </c>
       <c r="D79">
-        <v>116.022903611</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.763078396</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>616082</v>
+        <v>6140803</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80">
-        <v>-31.924002425000001</v>
+        <v>-32.139502155999999</v>
       </c>
       <c r="D80">
-        <v>115.92193885899999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.764091677</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>616084</v>
+        <v>6140804</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81">
-        <v>-31.877702540000001</v>
+        <v>-32.145769536000003</v>
       </c>
       <c r="D81">
-        <v>115.95952564</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.759278291</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>616086</v>
+        <v>6140805</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82">
-        <v>-31.900081093000001</v>
+        <v>-32.140391358999999</v>
       </c>
       <c r="D82">
-        <v>116.007611462</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.763698003</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>616087</v>
+        <v>6140806</v>
       </c>
       <c r="B83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83">
-        <v>-31.94828296</v>
+        <v>-32.140058994999997</v>
       </c>
       <c r="D83">
-        <v>115.91931938</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.76199554599999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>616088</v>
+        <v>6140807</v>
       </c>
       <c r="B84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84">
-        <v>-31.862700963999998</v>
+        <v>-32.139802988</v>
       </c>
       <c r="D84">
-        <v>116.013984561</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.76533866699999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>616089</v>
+        <v>6141400</v>
       </c>
       <c r="B85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>-31.821230719999999</v>
+        <v>-32.277315371</v>
       </c>
       <c r="D85">
-        <v>116.12921548</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.69471735</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>616091</v>
+        <v>6141401</v>
       </c>
       <c r="B86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86">
-        <v>-32.038305649999998</v>
+        <v>-32.121294421000002</v>
       </c>
       <c r="D86">
-        <v>115.91732057</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.67884956499999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>616092</v>
+        <v>6141402</v>
       </c>
       <c r="B87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87">
-        <v>-32.078355232</v>
+        <v>-32.086346229</v>
       </c>
       <c r="D87">
-        <v>115.978799149</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.730668072</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>616099</v>
+        <v>6141403</v>
       </c>
       <c r="B88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88">
-        <v>-31.817711536000001</v>
+        <v>-32.159064072</v>
       </c>
       <c r="D88">
-        <v>116.01405090999999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.68062705299999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>6161013</v>
+        <v>6141404</v>
       </c>
       <c r="B89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89">
-        <v>-31.820768780000002</v>
+        <v>-32.213118074</v>
       </c>
       <c r="D89">
-        <v>116.1276349</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.68872790899999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>616178</v>
+        <v>6141405</v>
       </c>
       <c r="B90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>-31.883961190000001</v>
+        <v>-32.191800078999997</v>
       </c>
       <c r="D90">
-        <v>116.09479099000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.743558827</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>616189</v>
+        <v>6141406</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91">
-        <v>-31.751071324000002</v>
+        <v>-32.272430454000002</v>
       </c>
       <c r="D91">
-        <v>116.024830094</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.71357999600001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>6161989</v>
+        <v>6141407</v>
       </c>
       <c r="B92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92">
-        <v>-32.096312699999999</v>
+        <v>-32.172281793000003</v>
       </c>
       <c r="D92">
-        <v>116.017131529</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.77041565099999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>6162924</v>
+        <v>6141408</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93">
-        <v>-32.033500109999999</v>
+        <v>-32.166702141000002</v>
       </c>
       <c r="D93">
-        <v>116.00569905</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.675225066</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>6162925</v>
+        <v>6141409</v>
       </c>
       <c r="B94" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94">
-        <v>-31.876150470999999</v>
+        <v>-32.310380764999998</v>
       </c>
       <c r="D94">
-        <v>116.017298422</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.702273499</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>6163143</v>
+        <v>6141410</v>
       </c>
       <c r="B95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95">
-        <v>-31.87541667</v>
+        <v>-32.241411339000003</v>
       </c>
       <c r="D95">
-        <v>115.95690878000001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.70672572399999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>6163625</v>
+        <v>6141411</v>
       </c>
       <c r="B96" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C96">
-        <v>-31.800609914999999</v>
+        <v>-32.068487177000002</v>
       </c>
       <c r="D96">
-        <v>115.999476379</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.655646777</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>6163713</v>
+        <v>6141412</v>
       </c>
       <c r="B97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97">
-        <v>-31.952680231999999</v>
+        <v>-32.128542680000002</v>
       </c>
       <c r="D97">
-        <v>115.880203943</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.737652864</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>6164314</v>
+        <v>6141430</v>
       </c>
       <c r="B98" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98">
-        <v>-31.78947681</v>
+        <v>-32.353486619999998</v>
       </c>
       <c r="D98">
-        <v>116.00394692</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+        <v>115.737810827</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>6164462</v>
+        <v>6141431</v>
       </c>
       <c r="B99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99">
-        <v>-31.949030721</v>
+        <v>-32.271186513000004</v>
       </c>
       <c r="D99">
-        <v>115.91973172500001</v>
+        <v>115.71201080199999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>6141432</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>-32.274486441000001</v>
+      </c>
+      <c r="D100">
+        <v>115.702510809</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>6142828</v>
+      </c>
+      <c r="B101" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101">
+        <v>-32.151307950000003</v>
+      </c>
+      <c r="D101">
+        <v>115.763858168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>6142829</v>
+      </c>
+      <c r="B102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C102">
+        <v>-32.144290167000001</v>
+      </c>
+      <c r="D102">
+        <v>115.761121969</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>6142830</v>
+      </c>
+      <c r="B103" t="s">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>-32.140010476</v>
+      </c>
+      <c r="D103">
+        <v>115.762568716</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>6142831</v>
+      </c>
+      <c r="B104" t="s">
+        <v>2</v>
+      </c>
+      <c r="C104">
+        <v>-32.145119981999997</v>
+      </c>
+      <c r="D104">
+        <v>115.755597373</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>6142832</v>
+      </c>
+      <c r="B105" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105">
+        <v>-32.145058720999998</v>
+      </c>
+      <c r="D105">
+        <v>115.750296898</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>6142833</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106">
+        <v>-32.144971618</v>
+      </c>
+      <c r="D106">
+        <v>115.73969547</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>6142834</v>
+      </c>
+      <c r="B107" t="s">
+        <v>2</v>
+      </c>
+      <c r="C107">
+        <v>-32.150493318000002</v>
+      </c>
+      <c r="D107">
+        <v>115.758047946</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>6142835</v>
+      </c>
+      <c r="B108" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108">
+        <v>-32.155449447000002</v>
+      </c>
+      <c r="D108">
+        <v>115.763961329</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>6142836</v>
+      </c>
+      <c r="B109" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109">
+        <v>-32.159338089999999</v>
+      </c>
+      <c r="D109">
+        <v>115.763113511</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>6142837</v>
+      </c>
+      <c r="B110" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110">
+        <v>-32.163882868000002</v>
+      </c>
+      <c r="D110">
+        <v>115.762023415</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>6142838</v>
+      </c>
+      <c r="B111" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111">
+        <v>-32.180066463000003</v>
+      </c>
+      <c r="D111">
+        <v>115.74287148400001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>6142839</v>
+      </c>
+      <c r="B112" t="s">
+        <v>2</v>
+      </c>
+      <c r="C112">
+        <v>-32.172858415</v>
+      </c>
+      <c r="D112">
+        <v>115.75650358599999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>6142840</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
+      </c>
+      <c r="C113">
+        <v>-32.172650988000001</v>
+      </c>
+      <c r="D113">
+        <v>115.76756831199999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>6142841</v>
+      </c>
+      <c r="B114" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <v>-32.163157814999998</v>
+      </c>
+      <c r="D114">
+        <v>115.747016923</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>6142842</v>
+      </c>
+      <c r="B115" t="s">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>-32.153388327999998</v>
+      </c>
+      <c r="D115">
+        <v>115.755230547</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>6142843</v>
+      </c>
+      <c r="B116" t="s">
+        <v>2</v>
+      </c>
+      <c r="C116">
+        <v>-32.155789816000002</v>
+      </c>
+      <c r="D116">
+        <v>115.75268478700001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>6142876</v>
+      </c>
+      <c r="B117" t="s">
+        <v>2</v>
+      </c>
+      <c r="C117">
+        <v>-32.107617742000002</v>
+      </c>
+      <c r="D117">
+        <v>115.693569427</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>6142877</v>
+      </c>
+      <c r="B118" t="s">
+        <v>2</v>
+      </c>
+      <c r="C118">
+        <v>-32.110703833000002</v>
+      </c>
+      <c r="D118">
+        <v>115.763578259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>6142878</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <v>-32.079808139000001</v>
+      </c>
+      <c r="D119">
+        <v>115.732652942</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>6142879</v>
+      </c>
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120">
+        <v>-32.103801263999998</v>
+      </c>
+      <c r="D120">
+        <v>115.736900898</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>6142880</v>
+      </c>
+      <c r="B121" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121">
+        <v>-32.071320587999999</v>
+      </c>
+      <c r="D121">
+        <v>115.682813321</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>6142881</v>
+      </c>
+      <c r="B122" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122">
+        <v>-32.132760543000003</v>
+      </c>
+      <c r="D122">
+        <v>115.711228404</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>6142882</v>
+      </c>
+      <c r="B123" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123">
+        <v>-32.088969908999999</v>
+      </c>
+      <c r="D123">
+        <v>115.751180955</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>6142883</v>
+      </c>
+      <c r="B124" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>-32.137772667999997</v>
+      </c>
+      <c r="D124">
+        <v>115.675749878</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>6142884</v>
+      </c>
+      <c r="B125" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125">
+        <v>-32.106617317999998</v>
+      </c>
+      <c r="D125">
+        <v>115.719769818</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>6142885</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126">
+        <v>-32.120796734999999</v>
+      </c>
+      <c r="D126">
+        <v>115.739655864</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>6142954</v>
+      </c>
+      <c r="B127" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127">
+        <v>-32.275105732999997</v>
+      </c>
+      <c r="D127">
+        <v>115.715867523</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>6142955</v>
+      </c>
+      <c r="B128" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <v>-32.256652029000001</v>
+      </c>
+      <c r="D128">
+        <v>115.75024587199999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>6142956</v>
+      </c>
+      <c r="B129" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129">
+        <v>-32.220266807000002</v>
+      </c>
+      <c r="D129">
+        <v>115.75793843300001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>6142957</v>
+      </c>
+      <c r="B130" t="s">
+        <v>2</v>
+      </c>
+      <c r="C130">
+        <v>-32.205789633999999</v>
+      </c>
+      <c r="D130">
+        <v>115.769095092</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>6142958</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2</v>
+      </c>
+      <c r="C131">
+        <v>-32.139657020999998</v>
+      </c>
+      <c r="D131">
+        <v>115.765171</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>6142959</v>
+      </c>
+      <c r="B132" t="s">
+        <v>2</v>
+      </c>
+      <c r="C132">
+        <v>-32.139546115000002</v>
+      </c>
+      <c r="D132">
+        <v>115.763974461</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>6142960</v>
+      </c>
+      <c r="B133" t="s">
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <v>-32.139141909999999</v>
+      </c>
+      <c r="D133">
+        <v>115.762304794</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>6142961</v>
+      </c>
+      <c r="B134" t="s">
+        <v>2</v>
+      </c>
+      <c r="C134">
+        <v>-32.139264445999999</v>
+      </c>
+      <c r="D134">
+        <v>115.76099908800001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>6142962</v>
+      </c>
+      <c r="B135" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135">
+        <v>-32.139827699999998</v>
+      </c>
+      <c r="D135">
+        <v>115.761404954</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>6142963</v>
+      </c>
+      <c r="B136" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136">
+        <v>-32.276016060000003</v>
+      </c>
+      <c r="D136">
+        <v>115.719347962</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>6142964</v>
+      </c>
+      <c r="B137" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137">
+        <v>-32.248486266999997</v>
+      </c>
+      <c r="D137">
+        <v>115.75550581500001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>6142965</v>
+      </c>
+      <c r="B138" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>-32.136481117999999</v>
+      </c>
+      <c r="D138">
+        <v>115.745844601</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>6142966</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139">
+        <v>-32.226458454000003</v>
+      </c>
+      <c r="D139">
+        <v>115.692123205</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>6142967</v>
+      </c>
+      <c r="B140" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140">
+        <v>-32.186900758</v>
+      </c>
+      <c r="D140">
+        <v>115.676247875</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>6142968</v>
+      </c>
+      <c r="B141" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141">
+        <v>-32.160219306999998</v>
+      </c>
+      <c r="D141">
+        <v>115.669486552</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>6142969</v>
+      </c>
+      <c r="B142" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142">
+        <v>-32.161968438999999</v>
+      </c>
+      <c r="D142">
+        <v>115.661709301</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>6142970</v>
+      </c>
+      <c r="B143" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143">
+        <v>-32.154537638999997</v>
+      </c>
+      <c r="D143">
+        <v>115.693851385</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>6142971</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2</v>
+      </c>
+      <c r="C144">
+        <v>-32.152352958999998</v>
+      </c>
+      <c r="D144">
+        <v>115.72016838499999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>6142972</v>
+      </c>
+      <c r="B145" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145">
+        <v>-32.146466224000001</v>
+      </c>
+      <c r="D145">
+        <v>115.756734788</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>6142973</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2</v>
+      </c>
+      <c r="C146">
+        <v>-32.170689052999997</v>
+      </c>
+      <c r="D146">
+        <v>115.762493428</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>6142974</v>
+      </c>
+      <c r="B147" t="s">
+        <v>2</v>
+      </c>
+      <c r="C147">
+        <v>-32.197551832000002</v>
+      </c>
+      <c r="D147">
+        <v>115.719843626</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>6142975</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148">
+        <v>-32.209837055000001</v>
+      </c>
+      <c r="D148">
+        <v>115.759576271</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>6142976</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149">
+        <v>-32.238920268000001</v>
+      </c>
+      <c r="D149">
+        <v>115.751422662</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>6142977</v>
+      </c>
+      <c r="B150" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150">
+        <v>-32.256486783</v>
+      </c>
+      <c r="D150">
+        <v>115.740874572</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>6142978</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151">
+        <v>-32.262387908000001</v>
+      </c>
+      <c r="D151">
+        <v>115.71418877399999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>6142979</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152">
+        <v>-32.254151135999997</v>
+      </c>
+      <c r="D152">
+        <v>115.684295647</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>6142980</v>
+      </c>
+      <c r="B153" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153">
+        <v>-32.229504706999997</v>
+      </c>
+      <c r="D153">
+        <v>115.697980027</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>6142981</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154">
+        <v>-32.198581773999997</v>
+      </c>
+      <c r="D154">
+        <v>115.68484153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>6142982</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>-32.157744698000002</v>
+      </c>
+      <c r="D155">
+        <v>115.682130625</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>6142983</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156">
+        <v>-32.248218041999998</v>
+      </c>
+      <c r="D156">
+        <v>115.712541575</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>6142984</v>
+      </c>
+      <c r="B157" t="s">
+        <v>2</v>
+      </c>
+      <c r="C157">
+        <v>-32.182789221</v>
+      </c>
+      <c r="D157">
+        <v>115.73910039499999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>6142985</v>
+      </c>
+      <c r="B158" t="s">
+        <v>2</v>
+      </c>
+      <c r="C158">
+        <v>-32.308824000999998</v>
+      </c>
+      <c r="D158">
+        <v>115.70879608200001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>6142986</v>
+      </c>
+      <c r="B159" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159">
+        <v>-32.336932527999998</v>
+      </c>
+      <c r="D159">
+        <v>115.72217755200001</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>6142987</v>
+      </c>
+      <c r="B160" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160">
+        <v>-32.254684758000003</v>
+      </c>
+      <c r="D160">
+        <v>115.740177589</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>6142988</v>
+      </c>
+      <c r="B161" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161">
+        <v>-32.215283460000002</v>
+      </c>
+      <c r="D161">
+        <v>115.696623</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>6142989</v>
+      </c>
+      <c r="B162" t="s">
+        <v>2</v>
+      </c>
+      <c r="C162">
+        <v>-32.198581773999997</v>
+      </c>
+      <c r="D162">
+        <v>115.68484153</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>6142990</v>
+      </c>
+      <c r="B163" t="s">
+        <v>2</v>
+      </c>
+      <c r="C163">
+        <v>-32.139387691000003</v>
+      </c>
+      <c r="D163">
+        <v>115.652985343</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>6144401</v>
+      </c>
+      <c r="B164" t="s">
+        <v>2</v>
+      </c>
+      <c r="C164">
+        <v>-32.250795482000001</v>
+      </c>
+      <c r="D164">
+        <v>115.728331977</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>6144466</v>
+      </c>
+      <c r="B165" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165">
+        <v>-32.197784099000003</v>
+      </c>
+      <c r="D165">
+        <v>115.765882315</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>6144467</v>
+      </c>
+      <c r="B166" t="s">
+        <v>2</v>
+      </c>
+      <c r="C166">
+        <v>-32.200103183000003</v>
+      </c>
+      <c r="D166">
+        <v>115.740660707</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>6144468</v>
+      </c>
+      <c r="B167" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167">
+        <v>-32.248688672999997</v>
+      </c>
+      <c r="D167">
+        <v>115.739527946</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>6147030</v>
+      </c>
+      <c r="B168" t="s">
+        <v>2</v>
+      </c>
+      <c r="C168">
+        <v>-32.156586550999997</v>
+      </c>
+      <c r="D168">
+        <v>115.70274002399999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>6147031</v>
+      </c>
+      <c r="B169" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169">
+        <v>-32.250786462999997</v>
+      </c>
+      <c r="D169">
+        <v>115.728332103</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>6147034</v>
+      </c>
+      <c r="B170" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170">
+        <v>-32.262387908000001</v>
+      </c>
+      <c r="D170">
+        <v>115.71418877399999</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>6147035</v>
+      </c>
+      <c r="B171" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>-32.200106294000001</v>
+      </c>
+      <c r="D171">
+        <v>115.74066512</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>6163718</v>
+      </c>
+      <c r="B172" t="s">
+        <v>2</v>
+      </c>
+      <c r="C172">
+        <v>-32.133485937000003</v>
+      </c>
+      <c r="D172">
+        <v>115.746723092</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40330F1-E7B6-418F-AE7B-0C3027927FC8}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>6147030</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>-32.156600179999998</v>
+      </c>
+      <c r="D1">
+        <v>115.70272919999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>6147031</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-32.250800060000003</v>
+      </c>
+      <c r="D2">
+        <v>115.7283213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>6147032</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-32.19228159</v>
+      </c>
+      <c r="D3">
+        <v>115.74524959999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>6147033</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-32.272864929999997</v>
+      </c>
+      <c r="D4">
+        <v>115.70268040000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6147034</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-32.262401539999999</v>
+      </c>
+      <c r="D5">
+        <v>115.714178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6147035</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>-32.200119899999997</v>
+      </c>
+      <c r="D6">
+        <v>115.7406544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6147036</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>-32.157431269999996</v>
+      </c>
+      <c r="D7">
+        <v>115.67930389999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6147037</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>-32.186697510000002</v>
+      </c>
+      <c r="D8">
+        <v>115.7598478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>